<commit_message>
fixed bug when backing removes value of field
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1577,103 +1577,9 @@
         <v>?</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26">
-        <v>71167</v>
-      </c>
-      <c r="B26" t="str">
-        <v>06DS8246BC3200</v>
-      </c>
-      <c r="C26" t="str">
-        <v>24389</v>
-      </c>
-      <c r="D26" t="str">
-        <v>OPEN</v>
-      </c>
-      <c r="E26" t="str">
-        <v>2</v>
-      </c>
-      <c r="F26" t="str">
-        <v>BAD</v>
-      </c>
-      <c r="G26" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="H26" t="str">
-        <v>NO</v>
-      </c>
-      <c r="I26" t="str">
-        <v>this is amazing!</v>
-      </c>
-      <c r="J26" t="str">
-        <v>dev</v>
-      </c>
-      <c r="K26" t="str">
-        <v>8/12/2022</v>
-      </c>
-      <c r="L26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M26" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="N26" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="O26" t="str">
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27">
-        <v>71168</v>
-      </c>
-      <c r="B27" t="str">
-        <v>06DSTESTBC3200</v>
-      </c>
-      <c r="C27" t="str">
-        <v>42379</v>
-      </c>
-      <c r="D27" t="str">
-        <v>208</v>
-      </c>
-      <c r="E27" t="str">
-        <v>2</v>
-      </c>
-      <c r="F27" t="str">
-        <v>GOOD</v>
-      </c>
-      <c r="G27" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="H27" t="str">
-        <v>NO</v>
-      </c>
-      <c r="I27" t="str">
-        <v/>
-      </c>
-      <c r="J27" t="str">
-        <v>dev</v>
-      </c>
-      <c r="K27" t="str">
-        <v>8/12/2022</v>
-      </c>
-      <c r="L27" t="b">
-        <v>0</v>
-      </c>
-      <c r="M27" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="N27" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="O27" t="str">
-        <v>YES</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lower-cased username and password on login
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1577,9 +1577,103 @@
         <v>?</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26">
+        <v>71278</v>
+      </c>
+      <c r="B26" t="str">
+        <v>06DF3136AA3600</v>
+      </c>
+      <c r="C26" t="str">
+        <v>3600J03031</v>
+      </c>
+      <c r="D26" t="str">
+        <v>460</v>
+      </c>
+      <c r="E26" t="str">
+        <v>?</v>
+      </c>
+      <c r="F26" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G26" t="str">
+        <v>NA</v>
+      </c>
+      <c r="H26" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I26" t="str">
+        <v/>
+      </c>
+      <c r="J26" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K26" t="str">
+        <v>8/31/2022</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N26" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O26" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>71279</v>
+      </c>
+      <c r="B27" t="str">
+        <v>JAS0N</v>
+      </c>
+      <c r="C27" t="str">
+        <v>DRFDWR</v>
+      </c>
+      <c r="D27" t="str">
+        <v>460</v>
+      </c>
+      <c r="E27" t="str">
+        <v>2</v>
+      </c>
+      <c r="F27" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G27" t="str">
+        <v>N/A23345</v>
+      </c>
+      <c r="H27" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I27" t="str">
+        <v>Jgyjgygujguj</v>
+      </c>
+      <c r="J27" t="str">
+        <v>west</v>
+      </c>
+      <c r="K27" t="str">
+        <v>8/31/2022</v>
+      </c>
+      <c r="L27" t="b">
+        <v>0</v>
+      </c>
+      <c r="M27" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N27" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O27" t="str">
+        <v>?</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wip -> motorshop paper
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1629,31 +1629,31 @@
         <v>71279</v>
       </c>
       <c r="B27" t="str">
-        <v>JAS0N</v>
+        <v>06D3136CC3600</v>
       </c>
       <c r="C27" t="str">
-        <v>DRFDWR</v>
+        <v>NO TAG</v>
       </c>
       <c r="D27" t="str">
         <v>460</v>
       </c>
       <c r="E27" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27" t="str">
         <v>GOOD</v>
       </c>
       <c r="G27" t="str">
-        <v>N/A23345</v>
+        <v>82523</v>
       </c>
       <c r="H27" t="str">
         <v>NO</v>
       </c>
       <c r="I27" t="str">
-        <v>Jgyjgygujguj</v>
+        <v/>
       </c>
       <c r="J27" t="str">
-        <v>west</v>
+        <v>ravi</v>
       </c>
       <c r="K27" t="str">
         <v>8/31/2022</v>
@@ -1668,12 +1668,294 @@
         <v>N/A</v>
       </c>
       <c r="O27" t="str">
-        <v>?</v>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>71280</v>
+      </c>
+      <c r="B28" t="str">
+        <v>O6E7265 310</v>
+      </c>
+      <c r="C28" t="str">
+        <v>6EABBC2L2H30</v>
+      </c>
+      <c r="D28" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E28" t="str">
+        <v>?</v>
+      </c>
+      <c r="F28" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G28" t="str">
+        <v>NA</v>
+      </c>
+      <c r="H28" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I28" t="str">
+        <v/>
+      </c>
+      <c r="J28" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K28" t="str">
+        <v>8/31/2022</v>
+      </c>
+      <c r="L28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M28" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N28" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O28" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>71281</v>
+      </c>
+      <c r="B29" t="str">
+        <v>NRA0400TFD</v>
+      </c>
+      <c r="C29" t="str">
+        <v>CT97E15052</v>
+      </c>
+      <c r="D29" t="str">
+        <v>460</v>
+      </c>
+      <c r="E29" t="str">
+        <v>0</v>
+      </c>
+      <c r="F29" t="str">
+        <v>?</v>
+      </c>
+      <c r="G29" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H29" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I29" t="str">
+        <v/>
+      </c>
+      <c r="J29" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K29" t="str">
+        <v>9/2/2022</v>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M29" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N29" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O29" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>71282</v>
+      </c>
+      <c r="B30" t="str">
+        <v>NRB 0400TFD</v>
+      </c>
+      <c r="C30" t="str">
+        <v>CT0400TFD</v>
+      </c>
+      <c r="D30" t="str">
+        <v>460</v>
+      </c>
+      <c r="E30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F30" t="str">
+        <v>BAD</v>
+      </c>
+      <c r="G30" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H30" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I30" t="str">
+        <v/>
+      </c>
+      <c r="J30" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K30" t="str">
+        <v>9/2/2022</v>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M30" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N30" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O30" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>71283</v>
+      </c>
+      <c r="B31" t="str">
+        <v>3DP3R12METFD</v>
+      </c>
+      <c r="C31" t="str">
+        <v>14162424R</v>
+      </c>
+      <c r="D31" t="str">
+        <v>460</v>
+      </c>
+      <c r="E31" t="str">
+        <v>1</v>
+      </c>
+      <c r="F31" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G31" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H31" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I31" t="str">
+        <v/>
+      </c>
+      <c r="J31" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K31" t="str">
+        <v>9/2/2022</v>
+      </c>
+      <c r="L31" t="b">
+        <v>0</v>
+      </c>
+      <c r="M31" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N31" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O31" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>71284</v>
+      </c>
+      <c r="B32" t="str">
+        <v>4RL2150ATSK</v>
+      </c>
+      <c r="C32" t="str">
+        <v>21F60072R</v>
+      </c>
+      <c r="D32" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E32" t="str">
+        <v>0</v>
+      </c>
+      <c r="F32" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G32" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H32" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I32" t="str">
+        <v/>
+      </c>
+      <c r="J32" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K32" t="str">
+        <v>9/2/2022</v>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
+      </c>
+      <c r="M32" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N32" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O32" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>71285</v>
+      </c>
+      <c r="B33" t="str">
+        <v>3DA3A060ETFC</v>
+      </c>
+      <c r="C33" t="str">
+        <v>ET06G02970R</v>
+      </c>
+      <c r="D33" t="str">
+        <v>208</v>
+      </c>
+      <c r="E33" t="str">
+        <v>0</v>
+      </c>
+      <c r="F33" t="str">
+        <v>BAD</v>
+      </c>
+      <c r="G33" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H33" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I33" t="str">
+        <v/>
+      </c>
+      <c r="J33" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K33" t="str">
+        <v>9/2/2022</v>
+      </c>
+      <c r="L33" t="b">
+        <v>0</v>
+      </c>
+      <c r="M33" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N33" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O33" t="str">
+        <v>NO</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wip -> motorshop pwk
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1953,9 +1953,902 @@
         <v>NO</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34">
+        <v>71286</v>
+      </c>
+      <c r="B34" t="str">
+        <v>06EY665E 103</v>
+      </c>
+      <c r="C34" t="str">
+        <v>0508UE0410</v>
+      </c>
+      <c r="D34" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E34" t="str">
+        <v>?</v>
+      </c>
+      <c r="F34" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G34" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H34" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I34" t="str">
+        <v/>
+      </c>
+      <c r="J34" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K34" t="str">
+        <v>9/6/2022</v>
+      </c>
+      <c r="L34" t="b">
+        <v>0</v>
+      </c>
+      <c r="M34" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N34" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O34" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>71287</v>
+      </c>
+      <c r="B35" t="str">
+        <v>06E26536A</v>
+      </c>
+      <c r="C35" t="str">
+        <v>65334NA2</v>
+      </c>
+      <c r="D35" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E35" t="str">
+        <v>?</v>
+      </c>
+      <c r="F35" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G35" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H35" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I35" t="str">
+        <v/>
+      </c>
+      <c r="J35" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K35" t="str">
+        <v>9/6/2022</v>
+      </c>
+      <c r="L35" t="b">
+        <v>0</v>
+      </c>
+      <c r="M35" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N35" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O35" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>71288</v>
+      </c>
+      <c r="B36" t="str">
+        <v>06EY77534A</v>
+      </c>
+      <c r="C36" t="str">
+        <v>67959NE2</v>
+      </c>
+      <c r="D36" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E36" t="str">
+        <v>?</v>
+      </c>
+      <c r="F36" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G36" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H36" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I36" t="str">
+        <v/>
+      </c>
+      <c r="J36" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K36" t="str">
+        <v>9/6/2022</v>
+      </c>
+      <c r="L36" t="b">
+        <v>0</v>
+      </c>
+      <c r="M36" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N36" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O36" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>71289</v>
+      </c>
+      <c r="B37" t="str">
+        <v>06ET265360</v>
+      </c>
+      <c r="C37" t="str">
+        <v>63522NA0</v>
+      </c>
+      <c r="D37" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E37" t="str">
+        <v>?</v>
+      </c>
+      <c r="F37" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G37" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H37" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I37" t="str">
+        <v/>
+      </c>
+      <c r="J37" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K37" t="str">
+        <v>9/6/2022</v>
+      </c>
+      <c r="L37" t="b">
+        <v>0</v>
+      </c>
+      <c r="M37" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N37" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O37" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>71290</v>
+      </c>
+      <c r="B38" t="str">
+        <v>06DX3376BC1200</v>
+      </c>
+      <c r="C38" t="str">
+        <v>66295NAE2</v>
+      </c>
+      <c r="D38" t="str">
+        <v>208</v>
+      </c>
+      <c r="E38" t="str">
+        <v>?</v>
+      </c>
+      <c r="F38" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G38" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H38" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I38" t="str">
+        <v/>
+      </c>
+      <c r="J38" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K38" t="str">
+        <v>9/6/2022</v>
+      </c>
+      <c r="L38" t="b">
+        <v>0</v>
+      </c>
+      <c r="M38" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N38" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O38" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>71291</v>
+      </c>
+      <c r="B39" t="str">
+        <v>DXS45</v>
+      </c>
+      <c r="C39" t="str">
+        <v>XXXXXXX</v>
+      </c>
+      <c r="D39" t="str">
+        <v>460</v>
+      </c>
+      <c r="E39" t="str">
+        <v>0</v>
+      </c>
+      <c r="F39" t="str">
+        <v>?</v>
+      </c>
+      <c r="G39" t="str">
+        <v>81605</v>
+      </c>
+      <c r="H39" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I39" t="str">
+        <v>Replaced Input - Brandon</v>
+      </c>
+      <c r="J39" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K39" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L39" t="b">
+        <v>0</v>
+      </c>
+      <c r="M39" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N39" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O39" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>71292</v>
+      </c>
+      <c r="B40" t="str">
+        <v>06E7299610</v>
+      </c>
+      <c r="C40" t="str">
+        <v>0305U00659</v>
+      </c>
+      <c r="D40" t="str">
+        <v>460</v>
+      </c>
+      <c r="E40" t="str">
+        <v>?</v>
+      </c>
+      <c r="F40" t="str">
+        <v>?</v>
+      </c>
+      <c r="G40" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H40" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I40" t="str">
+        <v/>
+      </c>
+      <c r="J40" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K40" t="str">
+        <v>9/6/2022</v>
+      </c>
+      <c r="L40" t="b">
+        <v>0</v>
+      </c>
+      <c r="M40" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N40" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O40" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>71293</v>
+      </c>
+      <c r="B41" t="str">
+        <v>06ET299660</v>
+      </c>
+      <c r="C41" t="str">
+        <v>69808ND2</v>
+      </c>
+      <c r="D41" t="str">
+        <v>460</v>
+      </c>
+      <c r="E41" t="str">
+        <v>?</v>
+      </c>
+      <c r="F41" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G41" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H41" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I41" t="str">
+        <v>Stator only</v>
+      </c>
+      <c r="J41" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K41" t="str">
+        <v>9/6/2022</v>
+      </c>
+      <c r="L41" t="b">
+        <v>0</v>
+      </c>
+      <c r="M41" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N41" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O41" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>71294</v>
+      </c>
+      <c r="B42" t="str">
+        <v>6DL3S2700TSK</v>
+      </c>
+      <c r="C42" t="str">
+        <v>NA</v>
+      </c>
+      <c r="D42" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E42" t="str">
+        <v>0</v>
+      </c>
+      <c r="F42" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G42" t="str">
+        <v>N/A82835</v>
+      </c>
+      <c r="H42" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I42" t="str">
+        <v/>
+      </c>
+      <c r="J42" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K42" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L42" t="b">
+        <v>0</v>
+      </c>
+      <c r="M42" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N42" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O42" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>71295</v>
+      </c>
+      <c r="B43" t="str">
+        <v>ONE 299 610</v>
+      </c>
+      <c r="C43" t="str">
+        <v>408 5J01412</v>
+      </c>
+      <c r="D43" t="str">
+        <v>460</v>
+      </c>
+      <c r="E43" t="str">
+        <v>0</v>
+      </c>
+      <c r="F43" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G43" t="str">
+        <v>82585</v>
+      </c>
+      <c r="H43" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I43" t="str">
+        <v>Stator only</v>
+      </c>
+      <c r="J43" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K43" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L43" t="b">
+        <v>0</v>
+      </c>
+      <c r="M43" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N43" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O43" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>71296</v>
+      </c>
+      <c r="B44" t="str">
+        <v>O6DG5373DC0600</v>
+      </c>
+      <c r="C44" t="str">
+        <v>1008U00036</v>
+      </c>
+      <c r="D44" t="str">
+        <v>460</v>
+      </c>
+      <c r="E44" t="str">
+        <v>2</v>
+      </c>
+      <c r="F44" t="str">
+        <v>?</v>
+      </c>
+      <c r="G44" t="str">
+        <v>N/A82920</v>
+      </c>
+      <c r="H44" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I44" t="str">
+        <v>E unl</v>
+      </c>
+      <c r="J44" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K44" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L44" t="b">
+        <v>0</v>
+      </c>
+      <c r="M44" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N44" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O44" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>71297</v>
+      </c>
+      <c r="B45" t="str">
+        <v>06DG5376DC0601</v>
+      </c>
+      <c r="C45" t="str">
+        <v>250465 15485</v>
+      </c>
+      <c r="D45" t="str">
+        <v>460</v>
+      </c>
+      <c r="E45" t="str">
+        <v>2</v>
+      </c>
+      <c r="F45" t="str">
+        <v>?</v>
+      </c>
+      <c r="G45" t="str">
+        <v>87942</v>
+      </c>
+      <c r="H45" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I45" t="str">
+        <v>2  e  unl</v>
+      </c>
+      <c r="J45" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K45" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L45" t="b">
+        <v>0</v>
+      </c>
+      <c r="M45" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N45" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O45" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>71298</v>
+      </c>
+      <c r="B46" t="str">
+        <v>06DG5376DC0601</v>
+      </c>
+      <c r="C46" t="str">
+        <v>300019 17066</v>
+      </c>
+      <c r="D46" t="str">
+        <v>460</v>
+      </c>
+      <c r="E46" t="str">
+        <v>2</v>
+      </c>
+      <c r="F46" t="str">
+        <v>?</v>
+      </c>
+      <c r="G46" t="str">
+        <v>87941</v>
+      </c>
+      <c r="H46" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I46" t="str">
+        <v>2 e unl</v>
+      </c>
+      <c r="J46" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K46" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L46" t="b">
+        <v>0</v>
+      </c>
+      <c r="M46" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N46" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O46" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>71299</v>
+      </c>
+      <c r="B47" t="str">
+        <v>O6DG5373DC0600</v>
+      </c>
+      <c r="C47" t="str">
+        <v>2607U03046</v>
+      </c>
+      <c r="D47" t="str">
+        <v>460</v>
+      </c>
+      <c r="E47" t="str">
+        <v>2</v>
+      </c>
+      <c r="F47" t="str">
+        <v>?</v>
+      </c>
+      <c r="G47" t="str">
+        <v>82943</v>
+      </c>
+      <c r="H47" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I47" t="str">
+        <v>2 e unl</v>
+      </c>
+      <c r="J47" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K47" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L47" t="b">
+        <v>0</v>
+      </c>
+      <c r="M47" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N47" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O47" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>71300</v>
+      </c>
+      <c r="B48" t="str">
+        <v>06DG53760601</v>
+      </c>
+      <c r="C48" t="str">
+        <v>NA</v>
+      </c>
+      <c r="D48" t="str">
+        <v>460</v>
+      </c>
+      <c r="E48" t="str">
+        <v>2</v>
+      </c>
+      <c r="F48" t="str">
+        <v>?</v>
+      </c>
+      <c r="G48" t="str">
+        <v>82944</v>
+      </c>
+      <c r="H48" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I48" t="str">
+        <v>2 e unl</v>
+      </c>
+      <c r="J48" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K48" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L48" t="b">
+        <v>0</v>
+      </c>
+      <c r="M48" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N48" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O48" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>71301</v>
+      </c>
+      <c r="B49" t="str">
+        <v>06DG5376DC0601</v>
+      </c>
+      <c r="C49" t="str">
+        <v>4619UD4187</v>
+      </c>
+      <c r="D49" t="str">
+        <v>460</v>
+      </c>
+      <c r="E49" t="str">
+        <v>2</v>
+      </c>
+      <c r="F49" t="str">
+        <v>?</v>
+      </c>
+      <c r="G49" t="str">
+        <v>82919</v>
+      </c>
+      <c r="H49" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I49" t="str">
+        <v>2 e unl</v>
+      </c>
+      <c r="J49" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K49" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L49" t="b">
+        <v>0</v>
+      </c>
+      <c r="M49" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N49" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O49" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>71302</v>
+      </c>
+      <c r="B50" t="str">
+        <v>O6EY675E 103</v>
+      </c>
+      <c r="C50" t="str">
+        <v>2605UE4569</v>
+      </c>
+      <c r="D50" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E50" t="str">
+        <v>0</v>
+      </c>
+      <c r="F50" t="str">
+        <v>BAD</v>
+      </c>
+      <c r="G50" t="str">
+        <v>82251</v>
+      </c>
+      <c r="H50" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I50" t="str">
+        <v/>
+      </c>
+      <c r="J50" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K50" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L50" t="b">
+        <v>0</v>
+      </c>
+      <c r="M50" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N50" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O50" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>71303</v>
+      </c>
+      <c r="B51" t="str">
+        <v>06CC675E2OO</v>
+      </c>
+      <c r="C51" t="str">
+        <v>1701J01641</v>
+      </c>
+      <c r="D51" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E51" t="str">
+        <v>0</v>
+      </c>
+      <c r="F51" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G51" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H51" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I51" t="str">
+        <v/>
+      </c>
+      <c r="J51" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K51" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L51" t="b">
+        <v>0</v>
+      </c>
+      <c r="M51" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N51" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O51" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>71304</v>
+      </c>
+      <c r="B52" t="str">
+        <v>6DL32700TSK</v>
+      </c>
+      <c r="C52" t="str">
+        <v>NA</v>
+      </c>
+      <c r="D52" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E52" t="str">
+        <v>0</v>
+      </c>
+      <c r="F52" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G52" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H52" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I52" t="str">
+        <v/>
+      </c>
+      <c r="J52" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K52" t="str">
+        <v>9/7/2022</v>
+      </c>
+      <c r="L52" t="b">
+        <v>0</v>
+      </c>
+      <c r="M52" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N52" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O52" t="str">
+        <v>NO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O33"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O52"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
linked lead tests to state
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2846,9 +2846,103 @@
         <v>NO</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53">
+        <v>71305</v>
+      </c>
+      <c r="B53" t="str">
+        <v>O6CC675E200</v>
+      </c>
+      <c r="C53" t="str">
+        <v>NA</v>
+      </c>
+      <c r="D53" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E53" t="str">
+        <v>0</v>
+      </c>
+      <c r="F53" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G53" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H53" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I53" t="str">
+        <v/>
+      </c>
+      <c r="J53" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K53" t="str">
+        <v>9/8/2022</v>
+      </c>
+      <c r="L53" t="b">
+        <v>0</v>
+      </c>
+      <c r="M53" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N53" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O53" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>71306</v>
+      </c>
+      <c r="B54" t="str">
+        <v>6M11 40X AWM D P</v>
+      </c>
+      <c r="C54" t="str">
+        <v>21B 43024 M</v>
+      </c>
+      <c r="D54" t="str">
+        <v>380 420 YY</v>
+      </c>
+      <c r="E54" t="str">
+        <v>0</v>
+      </c>
+      <c r="F54" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G54" t="str">
+        <v>82916</v>
+      </c>
+      <c r="H54" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I54" t="str">
+        <v/>
+      </c>
+      <c r="J54" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K54" t="str">
+        <v>9/8/2022</v>
+      </c>
+      <c r="L54" t="b">
+        <v>0</v>
+      </c>
+      <c r="M54" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N54" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O54" t="str">
+        <v>NO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O52"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O54"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated yes/ no selector to deselect if the same thing is pressed 2x
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2940,9 +2940,150 @@
         <v>NO</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55">
+        <v>71307</v>
+      </c>
+      <c r="B55" t="str">
+        <v>4MK1 35X AWM D P</v>
+      </c>
+      <c r="C55" t="str">
+        <v>21D 57594 M</v>
+      </c>
+      <c r="D55" t="str">
+        <v>380 420YY</v>
+      </c>
+      <c r="E55" t="str">
+        <v>0</v>
+      </c>
+      <c r="F55" t="str">
+        <v>?</v>
+      </c>
+      <c r="G55" t="str">
+        <v>82915</v>
+      </c>
+      <c r="H55" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I55" t="str">
+        <v/>
+      </c>
+      <c r="J55" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K55" t="str">
+        <v>9/8/2022</v>
+      </c>
+      <c r="L55" t="b">
+        <v>0</v>
+      </c>
+      <c r="M55" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N55" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O55" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>71308</v>
+      </c>
+      <c r="B56" t="str">
+        <v>O6DE5379DC1900</v>
+      </c>
+      <c r="C56" t="str">
+        <v>3609UD8512</v>
+      </c>
+      <c r="D56" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E56" t="str">
+        <v>2</v>
+      </c>
+      <c r="F56" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G56" t="str">
+        <v>82939</v>
+      </c>
+      <c r="H56" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I56" t="str">
+        <v/>
+      </c>
+      <c r="J56" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K56" t="str">
+        <v>9/8/2022</v>
+      </c>
+      <c r="L56" t="b">
+        <v>0</v>
+      </c>
+      <c r="M56" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N56" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O56" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>71309</v>
+      </c>
+      <c r="B57" t="str">
+        <v>O6DG5373DC0600</v>
+      </c>
+      <c r="C57" t="str">
+        <v>4307U00575</v>
+      </c>
+      <c r="D57" t="str">
+        <v>460</v>
+      </c>
+      <c r="E57" t="str">
+        <v>2</v>
+      </c>
+      <c r="F57" t="str">
+        <v>?</v>
+      </c>
+      <c r="G57" t="str">
+        <v>82940</v>
+      </c>
+      <c r="H57" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I57" t="str">
+        <v>2 s HD e unl</v>
+      </c>
+      <c r="J57" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K57" t="str">
+        <v>9/8/2022</v>
+      </c>
+      <c r="L57" t="b">
+        <v>0</v>
+      </c>
+      <c r="M57" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N57" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O57" t="str">
+        <v>NO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O54"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O57"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created toolbar to savepapers and select new ones
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3081,9 +3081,56 @@
         <v>NO</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58">
+        <v>71310</v>
+      </c>
+      <c r="B58" t="str">
+        <v>6002SC H</v>
+      </c>
+      <c r="C58" t="str">
+        <v>0282295</v>
+      </c>
+      <c r="D58" t="str">
+        <v>460</v>
+      </c>
+      <c r="E58" t="str">
+        <v>?</v>
+      </c>
+      <c r="F58" t="str">
+        <v>?</v>
+      </c>
+      <c r="G58" t="str">
+        <v>82480</v>
+      </c>
+      <c r="H58" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I58" t="str">
+        <v/>
+      </c>
+      <c r="J58" t="str">
+        <v>romel</v>
+      </c>
+      <c r="K58" t="str">
+        <v>9/9/2022</v>
+      </c>
+      <c r="L58" t="b">
+        <v>0</v>
+      </c>
+      <c r="M58" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N58" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O58" t="str">
+        <v>?</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O57"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O58"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created overlay for when data does not exist
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3128,9 +3128,103 @@
         <v>?</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59">
+        <v>71311</v>
+      </c>
+      <c r="B59" t="str">
+        <v>O6E3575 661</v>
+      </c>
+      <c r="C59" t="str">
+        <v>0920UE9854</v>
+      </c>
+      <c r="D59" t="str">
+        <v>460</v>
+      </c>
+      <c r="E59" t="str">
+        <v>2</v>
+      </c>
+      <c r="F59" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G59" t="str">
+        <v>82921</v>
+      </c>
+      <c r="H59" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I59" t="str">
+        <v>2 e unl</v>
+      </c>
+      <c r="J59" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K59" t="str">
+        <v>9/9/2022</v>
+      </c>
+      <c r="L59" t="b">
+        <v>0</v>
+      </c>
+      <c r="M59" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N59" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O59" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>71312</v>
+      </c>
+      <c r="B60" t="str">
+        <v>O6E3575661</v>
+      </c>
+      <c r="C60" t="str">
+        <v>5015UE6053</v>
+      </c>
+      <c r="D60" t="str">
+        <v>460</v>
+      </c>
+      <c r="E60" t="str">
+        <v>2</v>
+      </c>
+      <c r="F60" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G60" t="str">
+        <v>82923</v>
+      </c>
+      <c r="H60" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I60" t="str">
+        <v>2 e unl</v>
+      </c>
+      <c r="J60" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K60" t="str">
+        <v>9/9/2022</v>
+      </c>
+      <c r="L60" t="b">
+        <v>0</v>
+      </c>
+      <c r="M60" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N60" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O60" t="str">
+        <v>NO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O58"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O60"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified get/p1 to load most recent on NAN/ -1 values
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3269,9 +3269,56 @@
         <v>NO</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62">
+        <v>71314</v>
+      </c>
+      <c r="B62" t="str">
+        <v>DXS36</v>
+      </c>
+      <c r="C62" t="str">
+        <v>?</v>
+      </c>
+      <c r="D62" t="str">
+        <v>460</v>
+      </c>
+      <c r="E62" t="str">
+        <v>?</v>
+      </c>
+      <c r="F62" t="str">
+        <v>?</v>
+      </c>
+      <c r="G62" t="str">
+        <v>82863</v>
+      </c>
+      <c r="H62" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I62" t="str">
+        <v/>
+      </c>
+      <c r="J62" t="str">
+        <v>wes</v>
+      </c>
+      <c r="K62" t="str">
+        <v>9/12/2022</v>
+      </c>
+      <c r="L62" t="b">
+        <v>0</v>
+      </c>
+      <c r="M62" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N62" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O62" t="str">
+        <v>NO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O61"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O62"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
integrated status to display saved --also animated
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3316,9 +3316,150 @@
         <v>NO</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63">
+        <v>71315</v>
+      </c>
+      <c r="B63" t="str">
+        <v>6DH13500TSK</v>
+      </c>
+      <c r="C63" t="str">
+        <v>ET  00H01487S</v>
+      </c>
+      <c r="D63" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E63" t="str">
+        <v>?</v>
+      </c>
+      <c r="F63" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G63" t="str">
+        <v>82934</v>
+      </c>
+      <c r="H63" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I63" t="str">
+        <v/>
+      </c>
+      <c r="J63" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K63" t="str">
+        <v>9/12/2022</v>
+      </c>
+      <c r="L63" t="b">
+        <v>0</v>
+      </c>
+      <c r="M63" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N63" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O63" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>71316</v>
+      </c>
+      <c r="B64" t="str">
+        <v>6DP3R35METSK</v>
+      </c>
+      <c r="C64" t="str">
+        <v>21B62598R</v>
+      </c>
+      <c r="D64" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E64" t="str">
+        <v>?</v>
+      </c>
+      <c r="F64" t="str">
+        <v>GOOD</v>
+      </c>
+      <c r="G64" t="str">
+        <v>82926</v>
+      </c>
+      <c r="H64" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I64" t="str">
+        <v/>
+      </c>
+      <c r="J64" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K64" t="str">
+        <v>9/12/2022</v>
+      </c>
+      <c r="L64" t="b">
+        <v>0</v>
+      </c>
+      <c r="M64" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N64" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O64" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>71317</v>
+      </c>
+      <c r="B65" t="str">
+        <v>DXX36</v>
+      </c>
+      <c r="C65" t="str">
+        <v>3K9X067755</v>
+      </c>
+      <c r="D65" t="str">
+        <v>460</v>
+      </c>
+      <c r="E65" t="str">
+        <v>?</v>
+      </c>
+      <c r="F65" t="str">
+        <v>?</v>
+      </c>
+      <c r="G65" t="str">
+        <v>82867</v>
+      </c>
+      <c r="H65" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I65" t="str">
+        <v/>
+      </c>
+      <c r="J65" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K65" t="str">
+        <v>9/12/2022</v>
+      </c>
+      <c r="L65" t="b">
+        <v>0</v>
+      </c>
+      <c r="M65" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N65" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O65" t="str">
+        <v>NO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O62"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O65"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed error on import job save
</commit_message>
<xml_diff>
--- a/public/backup/jobs.xlsx
+++ b/public/backup/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3457,9 +3457,150 @@
         <v>NO</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66">
+        <v>71318</v>
+      </c>
+      <c r="B66" t="str">
+        <v>NA</v>
+      </c>
+      <c r="C66" t="str">
+        <v>NA</v>
+      </c>
+      <c r="D66" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E66" t="str">
+        <v>?</v>
+      </c>
+      <c r="F66" t="str">
+        <v>BAD</v>
+      </c>
+      <c r="G66" t="str">
+        <v>82628</v>
+      </c>
+      <c r="H66" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I66" t="str">
+        <v/>
+      </c>
+      <c r="J66" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K66" t="str">
+        <v>9/12/2022</v>
+      </c>
+      <c r="L66" t="b">
+        <v>0</v>
+      </c>
+      <c r="M66" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N66" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O66" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>71319</v>
+      </c>
+      <c r="B67" t="str">
+        <v>6DP3 3500 TSK</v>
+      </c>
+      <c r="C67" t="str">
+        <v>21G57035</v>
+      </c>
+      <c r="D67" t="str">
+        <v>MULTI</v>
+      </c>
+      <c r="E67" t="str">
+        <v>2</v>
+      </c>
+      <c r="F67" t="str">
+        <v>?</v>
+      </c>
+      <c r="G67" t="str">
+        <v>82932</v>
+      </c>
+      <c r="H67" t="str">
+        <v>NO</v>
+      </c>
+      <c r="I67" t="str">
+        <v/>
+      </c>
+      <c r="J67" t="str">
+        <v>ravi</v>
+      </c>
+      <c r="K67" t="str">
+        <v>9/12/2022</v>
+      </c>
+      <c r="L67" t="b">
+        <v>0</v>
+      </c>
+      <c r="M67" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N67" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O67" t="str">
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>70003</v>
+      </c>
+      <c r="B68" t="str">
+        <v>TEST06DS</v>
+      </c>
+      <c r="C68" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="D68" t="str">
+        <v>460</v>
+      </c>
+      <c r="E68" t="str">
+        <v>0</v>
+      </c>
+      <c r="F68" t="str">
+        <v>?</v>
+      </c>
+      <c r="G68" t="str">
+        <v>UU42839</v>
+      </c>
+      <c r="H68" t="str">
+        <v>true</v>
+      </c>
+      <c r="I68" t="str">
+        <v>false</v>
+      </c>
+      <c r="J68" t="str">
+        <v>spreadsheet</v>
+      </c>
+      <c r="K68" t="str">
+        <v>9/12/2022</v>
+      </c>
+      <c r="L68" t="b">
+        <v>0</v>
+      </c>
+      <c r="M68" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N68" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O68" t="str">
+        <v>?</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O65"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O68"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>